<commit_message>
react hot toste add
</commit_message>
<xml_diff>
--- a/public/Seller-add-by-partner-format.xlsx
+++ b/public/Seller-add-by-partner-format.xlsx
@@ -58,19 +58,19 @@
     <t xml:space="preserve">productCategories</t>
   </si>
   <si>
-    <t xml:space="preserve">Demo12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demo name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demo brand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seller@gmmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User@123</t>
+    <t xml:space="preserve">DEMO12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEMO NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEMO BRAND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEMO@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEMO@123</t>
   </si>
   <si>
     <t xml:space="preserve">pending</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">27ABCDE1234F1Z5</t>
   </si>
   <si>
-    <t xml:space="preserve">categories, clothing</t>
+    <t xml:space="preserve">Footwear,Fashion</t>
   </si>
 </sst>
 </file>
@@ -90,7 +90,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -132,6 +132,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
@@ -186,28 +193,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -404,111 +419,111 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="23.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="5" t="n">
         <v>45818</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="5" t="n">
         <v>45833</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="n">
+      <c r="G2" s="4" t="n">
         <v>9998887756</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1508,6 +1523,9 @@
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="DEMO@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>